<commit_message>
entering new json files
</commit_message>
<xml_diff>
--- a/Лист Microsoft Excel.xlsx
+++ b/Лист Microsoft Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\4. PROJECTS\6.VueJS\Khiva_tourists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111513D4-4EE5-45D3-A2A2-CF6664AC3823}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65252C04-1F9A-4446-8508-A82141F01F26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Minibus</t>
   </si>
@@ -124,6 +124,30 @@
   </si>
   <si>
     <t>Git</t>
+  </si>
+  <si>
+    <t>Umid Web Site Auto_drive, [09.09.2022 21:20]</t>
+  </si>
+  <si>
+    <t>3 bn 5  qala ekskursiya 45$</t>
+  </si>
+  <si>
+    <t>7 qala ekskursiya - 50$</t>
+  </si>
+  <si>
+    <t>10 qala - 55$</t>
+  </si>
+  <si>
+    <t>Umid Web Site Auto_drive, [09.09.2022 21:22]</t>
+  </si>
+  <si>
+    <t>Khiva,Buxoro, Samarqand, Toshkent  ekskursiya - 45$ 3 yil tajriba un</t>
+  </si>
+  <si>
+    <t>5 yil tajriba un 49$</t>
+  </si>
+  <si>
+    <t>10 yil tajriba un 59$</t>
   </si>
 </sst>
 </file>
@@ -193,9 +217,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -203,6 +224,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -484,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:O18"/>
+  <dimension ref="C1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,14 +519,15 @@
     <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="4" max="9" width="8.88671875" style="1"/>
     <col min="11" max="11" width="25.44140625" customWidth="1"/>
+    <col min="16" max="16" width="42.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -525,7 +550,7 @@
       <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>21</v>
       </c>
       <c r="N4">
@@ -534,8 +559,11 @@
       <c r="O4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
@@ -557,14 +585,17 @@
       <c r="I5" s="3">
         <v>39</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>2</v>
       </c>
       <c r="K5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
@@ -586,14 +617,17 @@
       <c r="I6" s="3">
         <v>89</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>3</v>
       </c>
       <c r="K6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
@@ -615,7 +649,7 @@
       <c r="I7" s="3">
         <v>89</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>4</v>
       </c>
       <c r="K7" t="s">
@@ -627,8 +661,11 @@
       <c r="M7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
@@ -644,14 +681,14 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="K8" s="7" t="s">
+      <c r="K8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="L8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
@@ -661,14 +698,17 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="L9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -684,8 +724,11 @@
       <c r="L10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
@@ -695,8 +738,11 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
@@ -718,54 +764,57 @@
       <c r="I12" s="3">
         <v>329</v>
       </c>
-    </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="P12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="8">
         <v>37</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="8">
         <v>37</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="8">
         <v>59</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="8">
         <v>79</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="8">
         <v>85</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="8">
         <v>229</v>
       </c>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="3:15" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="5" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="3:16" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="3">
@@ -788,7 +837,7 @@
       </c>
     </row>
     <row r="17" spans="3:9" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="3">
@@ -811,7 +860,7 @@
       </c>
     </row>
     <row r="18" spans="3:9" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="3">

</xml_diff>